<commit_message>
counter vowels full row test
</commit_message>
<xml_diff>
--- a/src/main/java/output/OutputFile.xlsx
+++ b/src/main/java/output/OutputFile.xlsx
@@ -40,25 +40,25 @@
     <t>Backness</t>
   </si>
   <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>Op-mid</t>
+  </si>
+  <si>
     <t>Open</t>
   </si>
   <si>
-    <t>Op-mid</t>
-  </si>
-  <si>
-    <t>Mid</t>
-  </si>
-  <si>
     <t>Cl-mid</t>
   </si>
   <si>
     <t>Close</t>
   </si>
   <si>
+    <t>Cent</t>
+  </si>
+  <si>
     <t>Front</t>
-  </si>
-  <si>
-    <t>Cent</t>
   </si>
   <si>
     <t>Back</t>
@@ -272,13 +272,13 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>11</v>
@@ -287,10 +287,10 @@
         <v>12</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>15</v>
@@ -301,6 +301,30 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>21.0</v>
       </c>
     </row>
     <row r="5">
@@ -438,6 +462,9 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E4" t="n">
+        <v>36.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1"/>
@@ -591,9 +618,6 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="n">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
all stats debug in progress
</commit_message>
<xml_diff>
--- a/src/main/java/output/OutputFile.xlsx
+++ b/src/main/java/output/OutputFile.xlsx
@@ -161,7 +161,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11.0"/>
@@ -209,11 +212,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -302,29 +308,29 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="n">
-        <v>17.0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2.0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>24.0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>20.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>39.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>21.0</v>
+      <c r="D4" t="n" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E4" t="n" s="2">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="F4" t="n" s="2">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="G4" t="n" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H4" t="n" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="I4" t="n" s="2">
+        <v>0.7666666666666667</v>
+      </c>
+      <c r="J4" t="n" s="2">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="K4" t="n" s="2">
+        <v>0.43333333333333335</v>
       </c>
     </row>
     <row r="5">
@@ -333,12 +339,60 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="D5" t="n" s="3">
+        <v>0.11333333333333333</v>
+      </c>
+      <c r="E5" t="n" s="3">
+        <v>0.006666666666666667</v>
+      </c>
+      <c r="F5" t="n" s="3">
+        <v>0.013333333333333334</v>
+      </c>
+      <c r="G5" t="n" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="H5" t="n" s="3">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="I5" t="n" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="J5" t="n" s="3">
+        <v>0.02666666666666667</v>
+      </c>
+      <c r="K5" t="n" s="3">
+        <v>0.14</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="D6" t="n" s="4">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="E6" t="n" s="4">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="F6" t="n" s="4">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="G6" t="n" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="H6" t="n" s="4">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="I6" t="n" s="4">
+        <v>1.3</v>
+      </c>
+      <c r="J6" t="n" s="4">
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="K6" t="n" s="4">
+        <v>0.7</v>
       </c>
     </row>
   </sheetData>
@@ -463,7 +517,7 @@
         <v>2</v>
       </c>
       <c r="E4" t="n">
-        <v>36.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="5">
@@ -472,12 +526,18 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E5" t="n">
+        <v>36.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>36.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor for implement NORMALITY output file
</commit_message>
<xml_diff>
--- a/src/main/java/output/OutputFile.xlsx
+++ b/src/main/java/output/OutputFile.xlsx
@@ -212,13 +212,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
@@ -339,28 +337,28 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="n" s="3">
+      <c r="D5" t="n" s="2">
         <v>0.11333333333333333</v>
       </c>
-      <c r="E5" t="n" s="3">
+      <c r="E5" t="n" s="2">
         <v>0.006666666666666667</v>
       </c>
-      <c r="F5" t="n" s="3">
+      <c r="F5" t="n" s="2">
         <v>0.013333333333333334</v>
       </c>
-      <c r="G5" t="n" s="3">
+      <c r="G5" t="n" s="2">
         <v>0.16</v>
       </c>
-      <c r="H5" t="n" s="3">
+      <c r="H5" t="n" s="2">
         <v>0.13333333333333333</v>
       </c>
-      <c r="I5" t="n" s="3">
+      <c r="I5" t="n" s="2">
         <v>0.26</v>
       </c>
-      <c r="J5" t="n" s="3">
+      <c r="J5" t="n" s="2">
         <v>0.02666666666666667</v>
       </c>
-      <c r="K5" t="n" s="3">
+      <c r="K5" t="n" s="2">
         <v>0.14</v>
       </c>
     </row>
@@ -370,28 +368,28 @@
       <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="n" s="4">
+      <c r="D6" t="n" s="2">
         <v>0.5666666666666667</v>
       </c>
-      <c r="E6" t="n" s="4">
+      <c r="E6" t="n" s="2">
         <v>0.03333333333333333</v>
       </c>
-      <c r="F6" t="n" s="4">
+      <c r="F6" t="n" s="2">
         <v>0.06666666666666667</v>
       </c>
-      <c r="G6" t="n" s="4">
+      <c r="G6" t="n" s="2">
         <v>0.8</v>
       </c>
-      <c r="H6" t="n" s="4">
+      <c r="H6" t="n" s="2">
         <v>0.6666666666666666</v>
       </c>
-      <c r="I6" t="n" s="4">
+      <c r="I6" t="n" s="2">
         <v>1.3</v>
       </c>
-      <c r="J6" t="n" s="4">
+      <c r="J6" t="n" s="2">
         <v>0.13333333333333333</v>
       </c>
-      <c r="K6" t="n" s="4">
+      <c r="K6" t="n" s="2">
         <v>0.7</v>
       </c>
     </row>
@@ -516,9 +514,6 @@
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="n">
-        <v>23.0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1"/>
@@ -526,18 +521,12 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="n">
-        <v>36.0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E6" t="n">
-        <v>36.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>